<commit_message>
added hatchery conditions table
</commit_message>
<xml_diff>
--- a/data/environmental/daily-measurements.xlsx
+++ b/data/environmental/daily-measurements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinebaird/Desktop/GitHub/polyIC-larvae/data/environmental/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/polyIC-larvae/data/environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADA8871-CBF6-6841-A6F8-4D653B4E04FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955A0B8D-C4F7-6940-9BC9-12FB69F7C3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00BD5C40-37F4-2C4B-83C9-57CC1D291904}"/>
+    <workbookView xWindow="30820" yWindow="-1460" windowWidth="18760" windowHeight="18760" xr2:uid="{00BD5C40-37F4-2C4B-83C9-57CC1D291904}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="30">
   <si>
     <t>PolyIC-tank1</t>
   </si>
@@ -79,9 +80,6 @@
     <t>initials</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>5K_1</t>
   </si>
   <si>
@@ -112,13 +110,22 @@
     <t>1K_10</t>
   </si>
   <si>
-    <t>FTR-Left</t>
-  </si>
-  <si>
-    <t>FTR-Right</t>
-  </si>
-  <si>
-    <t>GB</t>
+    <t>period</t>
+  </si>
+  <si>
+    <t>Day0-Day3</t>
+  </si>
+  <si>
+    <t>Day4-Day8</t>
+  </si>
+  <si>
+    <t>Day9-Day14</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>group</t>
   </si>
 </sst>
 </file>
@@ -492,16 +499,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0830F2-F0D8-2646-A72E-53EF0BB26B7B}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -524,12 +534,15 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>45572</v>
@@ -544,18 +557,21 @@
         <v>8.25</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>45572</v>
@@ -570,18 +586,21 @@
         <v>8.27</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>45573</v>
@@ -596,18 +615,21 @@
         <v>8.2799999999999994</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>45573</v>
@@ -622,18 +644,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>45573</v>
@@ -645,21 +670,24 @@
         <v>26.7</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>45573</v>
@@ -671,21 +699,24 @@
         <v>27.2</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>45574</v>
@@ -700,18 +731,21 @@
         <v>8.2899999999999991</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>45574</v>
@@ -726,18 +760,21 @@
         <v>8.32</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>45574</v>
@@ -752,7 +789,7 @@
         <v>8.4</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
@@ -760,10 +797,13 @@
       <c r="H10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>45574</v>
@@ -778,7 +818,7 @@
         <v>8.42</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
         <v>1</v>
@@ -786,10 +826,13 @@
       <c r="H11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>45575</v>
@@ -812,10 +855,13 @@
       <c r="H12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>45575</v>
@@ -838,10 +884,13 @@
       <c r="H13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>45575</v>
@@ -864,10 +913,13 @@
       <c r="H14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>45575</v>
@@ -890,10 +942,13 @@
       <c r="H15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>45575</v>
@@ -916,10 +971,13 @@
       <c r="H16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>45575</v>
@@ -942,10 +1000,13 @@
       <c r="H17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>45575</v>
@@ -968,10 +1029,13 @@
       <c r="H18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>45580</v>
@@ -994,10 +1058,13 @@
       <c r="H19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>45580</v>
@@ -1020,10 +1087,13 @@
       <c r="H20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>45580</v>
@@ -1046,10 +1116,13 @@
       <c r="H21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>45580</v>
@@ -1072,10 +1145,13 @@
       <c r="H22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>45580</v>
@@ -1098,10 +1174,13 @@
       <c r="H23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1">
         <v>45576</v>
@@ -1116,18 +1195,21 @@
         <v>8.36</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1">
         <v>45576</v>
@@ -1142,18 +1224,21 @@
         <v>8.35</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1">
         <v>45576</v>
@@ -1168,18 +1253,21 @@
         <v>8.34</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1">
         <v>45576</v>
@@ -1194,18 +1282,21 @@
         <v>8.33</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1">
         <v>45576</v>
@@ -1220,18 +1311,21 @@
         <v>8.34</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1">
         <v>45577</v>
@@ -1246,18 +1340,21 @@
         <v>8.27</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="1">
         <v>45577</v>
@@ -1272,18 +1369,21 @@
         <v>8.27</v>
       </c>
       <c r="F30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1">
         <v>45577</v>
@@ -1298,18 +1398,21 @@
         <v>8.26</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="1">
         <v>45577</v>
@@ -1324,18 +1427,21 @@
         <v>8.25</v>
       </c>
       <c r="F32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="1">
         <v>45577</v>
@@ -1350,18 +1456,21 @@
         <v>8.24</v>
       </c>
       <c r="F33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="1">
         <v>45578</v>
@@ -1376,18 +1485,21 @@
         <v>8.23</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="1">
         <v>45578</v>
@@ -1402,18 +1514,21 @@
         <v>8.24</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1">
         <v>45578</v>
@@ -1428,18 +1543,21 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="1">
         <v>45578</v>
@@ -1454,18 +1572,21 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1">
         <v>45578</v>
@@ -1480,18 +1601,21 @@
         <v>8.25</v>
       </c>
       <c r="F38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="1">
         <v>45579</v>
@@ -1506,18 +1630,21 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H39" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40" s="1">
         <v>45579</v>
@@ -1532,18 +1659,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H40" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="1">
         <v>45579</v>
@@ -1558,18 +1688,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1">
         <v>45579</v>
@@ -1584,18 +1717,21 @@
         <v>8.17</v>
       </c>
       <c r="F42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H42" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
         <v>45579</v>
@@ -1610,18 +1746,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="1">
         <v>45580</v>
@@ -1636,18 +1775,21 @@
         <v>8.1</v>
       </c>
       <c r="F44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" s="1">
         <v>45580</v>
@@ -1662,18 +1804,21 @@
         <v>8.1</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" s="1">
         <v>45580</v>
@@ -1688,18 +1833,21 @@
         <v>8.09</v>
       </c>
       <c r="F46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B47" s="1">
         <v>45580</v>
@@ -1714,18 +1862,21 @@
         <v>8.11</v>
       </c>
       <c r="F47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="1">
         <v>45580</v>
@@ -1740,18 +1891,21 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H48" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1">
         <v>45581</v>
@@ -1766,18 +1920,21 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="F49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H49" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1">
         <v>45581</v>
@@ -1792,18 +1949,21 @@
         <v>8.19</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H50" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" s="1">
         <v>45581</v>
@@ -1818,18 +1978,21 @@
         <v>8.19</v>
       </c>
       <c r="F51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H51" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1">
         <v>45581</v>
@@ -1844,18 +2007,21 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="F52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H52" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1">
         <v>45581</v>
@@ -1870,18 +2036,21 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H53" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="1">
         <v>45582</v>
@@ -1896,18 +2065,21 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H54" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1">
         <v>45582</v>
@@ -1922,18 +2094,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56" s="1">
         <v>45582</v>
@@ -1948,18 +2123,21 @@
         <v>8.18</v>
       </c>
       <c r="F56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G56" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H56" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" s="1">
         <v>45582</v>
@@ -1974,18 +2152,21 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H57" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="1">
         <v>45582</v>
@@ -2000,18 +2181,21 @@
         <v>8.19</v>
       </c>
       <c r="F58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H58" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" s="1">
         <v>45583</v>
@@ -2026,18 +2210,21 @@
         <v>8.1</v>
       </c>
       <c r="F59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" s="1">
         <v>45583</v>
@@ -2052,18 +2239,21 @@
         <v>8.11</v>
       </c>
       <c r="F60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H60" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" s="1">
         <v>45583</v>
@@ -2078,18 +2268,21 @@
         <v>8.11</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H61" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B62" s="1">
         <v>45583</v>
@@ -2104,18 +2297,21 @@
         <v>8.14</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H62" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B63" s="1">
         <v>45583</v>
@@ -2130,18 +2326,21 @@
         <v>8.14</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H63" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" s="1">
         <v>45584</v>
@@ -2156,18 +2355,21 @@
         <v>8.1300000000000008</v>
       </c>
       <c r="F64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H64" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="1">
         <v>45584</v>
@@ -2182,18 +2384,21 @@
         <v>8.1</v>
       </c>
       <c r="F65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H65" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="1">
         <v>45584</v>
@@ -2208,18 +2413,21 @@
         <v>8.09</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H66" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B67" s="1">
         <v>45584</v>
@@ -2234,18 +2442,21 @@
         <v>8.09</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H67" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B68" s="1">
         <v>45584</v>
@@ -2260,18 +2471,21 @@
         <v>8.06</v>
       </c>
       <c r="F68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H68" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B69" s="1">
         <v>45585</v>
@@ -2286,18 +2500,21 @@
         <v>8.1</v>
       </c>
       <c r="F69" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H69" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B70" s="1">
         <v>45585</v>
@@ -2312,18 +2529,21 @@
         <v>8.15</v>
       </c>
       <c r="F70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H70" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B71" s="1">
         <v>45585</v>
@@ -2338,18 +2558,21 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F71" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H71" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1">
         <v>45585</v>
@@ -2364,18 +2587,21 @@
         <v>8.15</v>
       </c>
       <c r="F72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H72" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B73" s="1">
         <v>45585</v>
@@ -2390,16 +2616,19 @@
         <v>8.15</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H73" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2424,8 +2653,11 @@
       <c r="H74" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -2450,8 +2682,11 @@
       <c r="H75" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -2476,8 +2711,11 @@
       <c r="H76" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -2502,8 +2740,11 @@
       <c r="H77" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -2528,8 +2769,11 @@
       <c r="H78" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2554,8 +2798,11 @@
       <c r="H79" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -2580,8 +2827,11 @@
       <c r="H80" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -2606,64 +2856,23 @@
       <c r="H81" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>25</v>
-      </c>
+      <c r="I81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>26</v>
-      </c>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>25</v>
-      </c>
-      <c r="B84" s="1">
-        <v>45671</v>
-      </c>
-      <c r="C84" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D84">
-        <v>10.4</v>
-      </c>
-      <c r="E84">
-        <v>7.87</v>
-      </c>
-      <c r="F84">
-        <v>24.49</v>
-      </c>
-      <c r="G84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>26</v>
-      </c>
-      <c r="B85" s="1">
-        <v>45671</v>
-      </c>
-      <c r="C85" s="2">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D85">
-        <v>11.5</v>
-      </c>
-      <c r="E85">
-        <v>8.11</v>
-      </c>
-      <c r="F85">
-        <v>27.89</v>
-      </c>
-      <c r="G85" t="s">
-        <v>27</v>
-      </c>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="1"/>
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="1"/>
+      <c r="C85" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>